<commit_message>
updated stats and results based on additions to corpora
</commit_message>
<xml_diff>
--- a/scripts/data/word_order/wals_word_order.xlsx
+++ b/scripts/data/word_order/wals_word_order.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13613" uniqueCount="5785">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13614" uniqueCount="5785">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -17497,8 +17497,8 @@
   </sheetPr>
   <dimension ref="A1:M1375"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A879" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E889" activeCellId="0" sqref="E889"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A432" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K444" activeCellId="0" sqref="K444"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -35512,6 +35512,9 @@
       <c r="J444" s="2" t="n">
         <v>7.5</v>
       </c>
+      <c r="K444" s="0" t="s">
+        <v>18</v>
+      </c>
       <c r="L444" s="2" t="s">
         <v>31</v>
       </c>
@@ -53267,10 +53270,10 @@
       <c r="J881" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="K881" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="L881" s="0" t="s">
+      <c r="K881" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L881" s="2" t="s">
         <v>32</v>
       </c>
       <c r="M881" s="2" t="s">

</xml_diff>